<commit_message>
added al filer for university
</commit_message>
<xml_diff>
--- a/3th course/МИЭП/лаба 3.xlsx
+++ b/3th course/МИЭП/лаба 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonkorolev/Documents/Универ/3th course/МИЭП/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonkorolev/Documents/university/3th course/МИЭП/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3259A9C2-1181-B543-B6E1-C37C32F079F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505AC0DE-59BA-0944-B646-9DDC4A0F3E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16880" xr2:uid="{25120A0A-33C2-3843-87D5-659787C98955}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{25120A0A-33C2-3843-87D5-659787C98955}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,11 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="10">
+  <futureMetadata name="XLRICHVALUE" count="11">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -111,8 +111,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="10">
+  <valueMetadata count="11">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -143,12 +150,15 @@
     <bk>
       <rc t="1" v="9"/>
     </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>t</t>
   </si>
@@ -221,13 +231,20 @@
   <si>
     <t>Нижняя граница</t>
   </si>
+  <si>
+    <t>Коэффициент автокорреляции первого порядка</t>
+  </si>
+  <si>
+    <t>&gt; 0,36 - сл. нулевая гипотеза о присутствии автокорреляции принимается</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -292,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,6 +347,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -345,6 +371,964 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Сравнение</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> фактических и расчетных значений</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Фактические значения</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B4D-4B47-BE6A-E728B4B0FE99}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Расчетные значения</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>89.244439999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81.16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.540000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76.31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1B4D-4B47-BE6A-E728B4B0FE99}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="35600383"/>
+        <c:axId val="35599487"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="35600383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35599487"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="35599487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35600383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,8 +1431,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1036320</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>101601</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1168401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -479,6 +1463,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1437640</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52B82953-07BD-C850-1CBD-F9DCCFC6525C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -525,7 +1545,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="10">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="11">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -566,6 +1586,10 @@
     <v>9</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -590,6 +1614,7 @@
   <rel r:id="rId8"/>
   <rel r:id="rId9"/>
   <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
 </richValueRels>
 </file>
 
@@ -910,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7061A82-CE97-D645-A779-6485A4BA3C66}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -999,8 +2024,8 @@
       <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5">
-        <f>(ABS(D2)/B2)*100</f>
+      <c r="I2" s="15">
+        <f>ABS(D2/B2*100)</f>
         <v>0.83951111111111409</v>
       </c>
       <c r="J2" s="5">
@@ -1053,8 +2078,8 @@
         <f>$D3*$D2</f>
         <v>-0.46844720000000512</v>
       </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I3:I10" si="3">(ABS(D3)/B3)*100</f>
+      <c r="I3" s="15">
+        <f t="shared" ref="I3:I10" si="3">ABS(D3/B3*100)</f>
         <v>0.71264367816092478</v>
       </c>
       <c r="J3" s="5">
@@ -1102,7 +2127,7 @@
         <f t="shared" ref="H4:H10" si="7">$D4*$D3</f>
         <v>0.62620000000000775</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="15">
         <f t="shared" si="3"/>
         <v>1.1882352941176531</v>
       </c>
@@ -1151,7 +2176,7 @@
         <f t="shared" si="7"/>
         <v>-1.6261000000000077</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="15">
         <f t="shared" si="3"/>
         <v>1.8720930232558133</v>
       </c>
@@ -1200,7 +2225,7 @@
         <f t="shared" si="7"/>
         <v>-1.2396999999999931</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="15">
         <f t="shared" si="3"/>
         <v>0.9390243902438975</v>
       </c>
@@ -1249,7 +2274,7 @@
         <f t="shared" si="7"/>
         <v>0.89319999999999278</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="15">
         <f t="shared" si="3"/>
         <v>1.4499999999999957</v>
       </c>
@@ -1298,7 +2323,7 @@
         <f t="shared" si="7"/>
         <v>-1.6935999999999878</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="15">
         <f t="shared" si="3"/>
         <v>1.8024691358024616</v>
       </c>
@@ -1347,7 +2372,7 @@
         <f t="shared" si="7"/>
         <v>0.116799999999997</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="15">
         <f t="shared" si="3"/>
         <v>0.10256410256410037</v>
       </c>
@@ -1396,7 +2421,7 @@
         <f t="shared" si="7"/>
         <v>-2.4799999999999652E-2</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="15">
         <f t="shared" si="3"/>
         <v>0.4078947368421082</v>
       </c>
@@ -1533,7 +2558,7 @@
         <v>73.702515758693551</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16" customHeight="1">
+    <row r="17" spans="1:17" ht="16" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1564,13 +2589,13 @@
         <v>72.102515758693542</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="D19" t="s">
         <v>5</v>
       </c>
@@ -1583,13 +2608,13 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="M20" s="6"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1597,9 +2622,11 @@
         <f>STDEV(D2:D10)</f>
         <v>1.0452230869585255</v>
       </c>
-      <c r="N23" s="6"/>
+      <c r="N23" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="24" spans="1:16" ht="68">
+    <row r="24" spans="1:17" ht="102" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>7</v>
       </c>
@@ -1607,12 +2634,24 @@
         <f>ABS(SUM(D2:D10)/COUNT(D2:D10))</f>
         <v>3.9511111111099556E-3</v>
       </c>
+      <c r="N24" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="O24" s="16">
+        <f>ABS(H11/E11)</f>
+        <v>0.39089467737428008</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="G17:J19"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="A15:C16"/>
+    <mergeCell ref="P24:Q24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>